<commit_message>
- Sequence ImportProduct - Modify Template.xlsx
</commit_message>
<xml_diff>
--- a/ smart-buy/Stuff/Template.xlsx
+++ b/ smart-buy/Stuff/Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="124">
   <si>
     <t>STT</t>
   </si>
@@ -33,355 +33,358 @@
     <t>BIỂU MẪU NHẬP GIÁ SẢN PHẨM</t>
   </si>
   <si>
+    <t>Gạo thơm Chợ Đào</t>
+  </si>
+  <si>
+    <t>Nếp thường</t>
+  </si>
+  <si>
+    <t>Bột mì Bình Đông</t>
+  </si>
+  <si>
+    <t>Thịt heo đùi</t>
+  </si>
+  <si>
+    <t>Thịt heo nạt lưng</t>
+  </si>
+  <si>
+    <t>Thịt heo ba rọi</t>
+  </si>
+  <si>
+    <t>Gan heo tươi</t>
+  </si>
+  <si>
+    <t>Thịt bò phi lê</t>
+  </si>
+  <si>
+    <t>Thịt bò đùi</t>
+  </si>
+  <si>
+    <t>Lạp xưởng vissan loại I</t>
+  </si>
+  <si>
+    <t>Thịt hộp Pate Vissan (hộp 170g)</t>
+  </si>
+  <si>
+    <t>Trứng vịt loại I</t>
+  </si>
+  <si>
+    <t>Dầu ăn tổng hợp Tường An</t>
+  </si>
+  <si>
+    <t>Tép đất (tôm đồng)</t>
+  </si>
+  <si>
+    <t>Gạo trắng thường</t>
+  </si>
+  <si>
+    <t>Mực ống tươi (8-10 con/kg)</t>
+  </si>
+  <si>
+    <t>Tôm khô loại I</t>
+  </si>
+  <si>
+    <t>Đậu phộng (cũ)loại I</t>
+  </si>
+  <si>
+    <t>Đậu xanh mỡ hột loại I</t>
+  </si>
+  <si>
+    <t>Đậu đen loại I</t>
+  </si>
+  <si>
+    <t>Đậu nành loại I</t>
+  </si>
+  <si>
+    <t>Rau muống</t>
+  </si>
+  <si>
+    <t>Cải bẹ xanh</t>
+  </si>
+  <si>
+    <t>Bắp cải Đà Lạt</t>
+  </si>
+  <si>
+    <t>Đậu Côve</t>
+  </si>
+  <si>
+    <t>Quýt Đường loại 1</t>
+  </si>
+  <si>
+    <t>Cam sành (4-5 trái/kg)</t>
+  </si>
+  <si>
+    <t>Tiêu hột đen loại I</t>
+  </si>
+  <si>
+    <t>Đường RE Biên Hoà (loại rời)</t>
+  </si>
+  <si>
+    <t>Đường tán (phên)</t>
+  </si>
+  <si>
+    <t>Đường kết tinh Mỹ Tho nội (ngà)</t>
+  </si>
+  <si>
+    <t>Sữa hộp Ông Thọ</t>
+  </si>
+  <si>
+    <t>Sữa DIELAC đỏ VN hộp 400gr</t>
+  </si>
+  <si>
+    <t>Sữa MEIJI Nhật hộp 400gr</t>
+  </si>
+  <si>
+    <t>Cà phê Moka loại I (hạt)</t>
+  </si>
+  <si>
+    <t>Coca Cola VN sản xuất (lon)</t>
+  </si>
+  <si>
+    <t>Bia Tiger SX tại VN (lon)</t>
+  </si>
+  <si>
+    <t>Bia HEINEKEN lon(thùng 24 lon)</t>
+  </si>
+  <si>
+    <t>KT nội trắng Việt Thắng khổ 1,15m</t>
+  </si>
+  <si>
+    <t>Vải thun màu khổ 1,6m</t>
+  </si>
+  <si>
+    <t>Áo sơ mi nữ ngắn tay</t>
+  </si>
+  <si>
+    <t>Giấy kẻ ngang 20 tờ (lớn)</t>
+  </si>
+  <si>
+    <t>Chợ Bình Tây</t>
+  </si>
+  <si>
+    <t>Viết Bic Sài Gòn</t>
+  </si>
+  <si>
+    <t>Giấy photo Bãi Bằng (70gr/m2)</t>
+  </si>
+  <si>
+    <t>sữa tươi tiệt trùng (VINAMILK) gói 220 ml</t>
+  </si>
+  <si>
+    <t>Nước suối La Vie (chai nhựa 1,25L)</t>
+  </si>
+  <si>
+    <t>Vải quần jean Thành Công khổ 1,6m</t>
+  </si>
+  <si>
+    <t>áo sơ mi nam Việt Thắng KT (dài tay)</t>
+  </si>
+  <si>
+    <t>Tập học sinh (100 trang)</t>
+  </si>
+  <si>
+    <t>Gạo trắng hạt dài thơm</t>
+  </si>
+  <si>
+    <t>Bia chai Sài Gòn xanh</t>
+  </si>
+  <si>
+    <t>Gà làm sẵn công nghiệp</t>
+  </si>
+  <si>
+    <t>Cá lóc (0,5kg/con)</t>
+  </si>
+  <si>
+    <t>Nếp Sáp</t>
+  </si>
+  <si>
+    <t>Thịt heo nạc đùi</t>
+  </si>
+  <si>
+    <t>Gà tam hoàng làm sẵn(con 1- 1.5 kg)</t>
+  </si>
+  <si>
+    <t>Cá lóc nuôi bè(0.5kg)</t>
+  </si>
+  <si>
+    <t>Tôm bạc(100/110 con/kg)</t>
+  </si>
+  <si>
+    <t>Tôm đất(tôm đồng)</t>
+  </si>
+  <si>
+    <t>Mực ống(8 - 10 con/kg)</t>
+  </si>
+  <si>
+    <t>Chả lụa(vissan)</t>
+  </si>
+  <si>
+    <t>Bí xanh</t>
+  </si>
+  <si>
+    <t>Cà chua</t>
+  </si>
+  <si>
+    <t>Cà rốt đà lạt</t>
+  </si>
+  <si>
+    <t>Khổ qua</t>
+  </si>
+  <si>
+    <t>Dưa leo</t>
+  </si>
+  <si>
+    <t>Xà lách Đà Lạt</t>
+  </si>
+  <si>
+    <t>Khoai tây Đà Lạt</t>
+  </si>
+  <si>
+    <t>Xoài cát Hòa Lộc(2 trái/kg)</t>
+  </si>
+  <si>
+    <t>Bưởi năm roi(trái 1kg)</t>
+  </si>
+  <si>
+    <t>Vải Calicot bông khổ 0.90m</t>
+  </si>
+  <si>
+    <t>Vải Tejin nội khổ 1.40m</t>
+  </si>
+  <si>
+    <t>Bia lon 333 Sài Gòn (thùng 24 lon)</t>
+  </si>
+  <si>
+    <t>Đường RE Biên Hòa (bịch 1 kg)</t>
+  </si>
+  <si>
+    <t>Mãng cầu(4-5 trái/kg)</t>
+  </si>
+  <si>
+    <t>Gạo tẻ trắng IR 64 25% tấm</t>
+  </si>
+  <si>
+    <t>Quýt tiểu loại 1</t>
+  </si>
+  <si>
+    <t>Táo khô(trung quốc)</t>
+  </si>
+  <si>
+    <t>Nho khô loại lớn</t>
+  </si>
+  <si>
+    <t>Hạt dưa</t>
+  </si>
+  <si>
+    <t>Mứt khoai thanh</t>
+  </si>
+  <si>
+    <t>Mứt dừa dẻo</t>
+  </si>
+  <si>
+    <t>Mứt me</t>
+  </si>
+  <si>
+    <t>Mứt bí tâm</t>
+  </si>
+  <si>
+    <t>Mứt gừng huế</t>
+  </si>
+  <si>
+    <t>Mứt hạt sen huế</t>
+  </si>
+  <si>
+    <t>Mứt mãng cầu</t>
+  </si>
+  <si>
+    <t>Táo trung quốc</t>
+  </si>
+  <si>
+    <t>Lê trung quốc</t>
+  </si>
+  <si>
+    <t>Nho tươi đỏ(mỹ)</t>
+  </si>
+  <si>
+    <t>Bánh hộp kinh đô 500 gr</t>
+  </si>
+  <si>
+    <t>Bánh hộp Danisa 453 gr</t>
+  </si>
+  <si>
+    <t>Bánh hộp Bibica (Biên Hòa) 350 gr</t>
+  </si>
+  <si>
+    <t>Trà sen loại 1</t>
+  </si>
+  <si>
+    <t>Nước ngọt Pepsi lon (Thùng 24 lon)</t>
+  </si>
+  <si>
+    <t>Nhãn tiêu</t>
+  </si>
+  <si>
+    <t>Đu Đủ</t>
+  </si>
+  <si>
+    <t>Tôm sú</t>
+  </si>
+  <si>
+    <t>Dưa hấu giống TL trái 3 kg</t>
+  </si>
+  <si>
+    <t>Thịt Vai</t>
+  </si>
+  <si>
+    <t>Thịt nách</t>
+  </si>
+  <si>
+    <t>Thịt cốt lếch</t>
+  </si>
+  <si>
+    <t>sườn già</t>
+  </si>
+  <si>
+    <t>chân giò</t>
+  </si>
+  <si>
+    <t>Dầu ăn tổng hợp Nakydaco (chai 1 lít)</t>
+  </si>
+  <si>
+    <t>Dầu ăn tổng hợp Neptune (chai 1 lít)</t>
+  </si>
+  <si>
+    <t>chả lụa cơ sở DÌ BẢY</t>
+  </si>
+  <si>
+    <t>Dầu ăn tổng hợp TƯỜNG AN (chai 1 lit)</t>
+  </si>
+  <si>
+    <t>Chợ Gò vấp</t>
+  </si>
+  <si>
+    <t>BigC Gò Vấp</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>Thóc tẻ thường</t>
   </si>
   <si>
-    <t>Gạo thơm Chợ Đào</t>
-  </si>
-  <si>
-    <t>Nếp thường</t>
-  </si>
-  <si>
-    <t>Bột mì Bình Đông</t>
-  </si>
-  <si>
-    <t>Thịt heo đùi</t>
-  </si>
-  <si>
-    <t>Thịt heo nạt lưng</t>
-  </si>
-  <si>
-    <t>Thịt heo ba rọi</t>
-  </si>
-  <si>
-    <t>Gan heo tươi</t>
-  </si>
-  <si>
-    <t>Thịt bò phi lê</t>
-  </si>
-  <si>
-    <t>Thịt bò đùi</t>
-  </si>
-  <si>
-    <t>Lạp xưởng vissan loại I</t>
-  </si>
-  <si>
-    <t>Thịt hộp Pate Vissan (hộp 170g)</t>
-  </si>
-  <si>
-    <t>Trứng gà công nghiệp loại I</t>
-  </si>
-  <si>
-    <t>Trứng vịt loại I</t>
-  </si>
-  <si>
-    <t>Dầu ăn tổng hợp Tường An</t>
-  </si>
-  <si>
-    <t>Tép đất (tôm đồng)</t>
-  </si>
-  <si>
-    <t>Gạo trắng thường</t>
-  </si>
-  <si>
-    <t>Mực ống tươi (8-10 con/kg)</t>
-  </si>
-  <si>
-    <t>Tôm khô loại I</t>
-  </si>
-  <si>
-    <t>Đậu phộng (cũ)loại I</t>
-  </si>
-  <si>
-    <t>Đậu xanh mỡ hột loại I</t>
-  </si>
-  <si>
-    <t>Đậu đen loại I</t>
-  </si>
-  <si>
-    <t>Đậu nành loại I</t>
-  </si>
-  <si>
-    <t>Rau muống</t>
-  </si>
-  <si>
-    <t>Cải bẹ xanh</t>
-  </si>
-  <si>
-    <t>Bắp cải Đà Lạt</t>
-  </si>
-  <si>
-    <t>Đậu Côve</t>
-  </si>
-  <si>
-    <t>Quýt Đường loại 1</t>
-  </si>
-  <si>
-    <t>Cam sành (4-5 trái/kg)</t>
-  </si>
-  <si>
-    <t>Tiêu hột đen loại I</t>
-  </si>
-  <si>
-    <t>Đường RE Biên Hoà (loại rời)</t>
-  </si>
-  <si>
-    <t>Đường tán (phên)</t>
-  </si>
-  <si>
-    <t>Đường kết tinh Mỹ Tho nội (ngà)</t>
-  </si>
-  <si>
-    <t>Sữa hộp Ông Thọ</t>
-  </si>
-  <si>
-    <t>Sữa DIELAC đỏ VN hộp 400gr</t>
-  </si>
-  <si>
-    <t>Sữa MEIJI Nhật hộp 400gr</t>
-  </si>
-  <si>
-    <t>Cà phê Moka loại I (hạt)</t>
-  </si>
-  <si>
-    <t>Coca Cola VN sản xuất (lon)</t>
-  </si>
-  <si>
-    <t>Bia Tiger SX tại VN (lon)</t>
-  </si>
-  <si>
-    <t>Bia HEINEKEN lon(thùng 24 lon)</t>
-  </si>
-  <si>
-    <t>KT nội trắng Việt Thắng khổ 1,15m</t>
-  </si>
-  <si>
-    <t>Vải thun màu khổ 1,6m</t>
-  </si>
-  <si>
-    <t>Áo sơ mi nữ ngắn tay</t>
-  </si>
-  <si>
-    <t>Giấy kẻ ngang 20 tờ (lớn)</t>
-  </si>
-  <si>
-    <t>Chợ Bình Tây</t>
-  </si>
-  <si>
-    <t>Viết Bic Sài Gòn</t>
-  </si>
-  <si>
-    <t>Giấy photo Bãi Bằng (70gr/m2)</t>
-  </si>
-  <si>
-    <t>sữa tươi tiệt trùng (VINAMILK) gói 220 ml</t>
-  </si>
-  <si>
-    <t>Nước suối La Vie (chai nhựa 1,25L)</t>
-  </si>
-  <si>
-    <t>Vải quần jean Thành Công khổ 1,6m</t>
-  </si>
-  <si>
-    <t>áo sơ mi nam Việt Thắng KT (dài tay)</t>
-  </si>
-  <si>
-    <t>Tập học sinh (100 trang)</t>
-  </si>
-  <si>
-    <t>Gạo trắng hạt dài thơm</t>
-  </si>
-  <si>
-    <t>Bia chai Sài Gòn xanh</t>
-  </si>
-  <si>
-    <t>Gà làm sẵn công nghiệp</t>
-  </si>
-  <si>
-    <t>Cá lóc (0,5kg/con)</t>
-  </si>
-  <si>
-    <t>Nếp Sáp</t>
-  </si>
-  <si>
-    <t>Thịt heo nạc đùi</t>
-  </si>
-  <si>
-    <t>Gà tam hoàng làm sẵn(con 1- 1.5 kg)</t>
-  </si>
-  <si>
-    <t>Cá lóc nuôi bè(0.5kg)</t>
-  </si>
-  <si>
-    <t>Tôm bạc(100/110 con/kg)</t>
-  </si>
-  <si>
-    <t>Tôm đất(tôm đồng)</t>
-  </si>
-  <si>
-    <t>Mực ống(8 - 10 con/kg)</t>
-  </si>
-  <si>
-    <t>Chả lụa(vissan)</t>
-  </si>
-  <si>
-    <t>Bí xanh</t>
-  </si>
-  <si>
-    <t>Cà chua</t>
-  </si>
-  <si>
-    <t>Cà rốt đà lạt</t>
-  </si>
-  <si>
-    <t>Khổ qua</t>
-  </si>
-  <si>
-    <t>Dưa leo</t>
-  </si>
-  <si>
-    <t>Xà lách Đà Lạt</t>
-  </si>
-  <si>
-    <t>Khoai tây Đà Lạt</t>
-  </si>
-  <si>
-    <t>Xoài cát Hòa Lộc(2 trái/kg)</t>
-  </si>
-  <si>
-    <t>Bưởi năm roi(trái 1kg)</t>
-  </si>
-  <si>
-    <t>Vải Calicot bông khổ 0.90m</t>
-  </si>
-  <si>
-    <t>Vải Tejin nội khổ 1.40m</t>
-  </si>
-  <si>
-    <t>Bia lon 333 Sài Gòn (thùng 24 lon)</t>
-  </si>
-  <si>
-    <t>Đường RE Biên Hòa (bịch 1 kg)</t>
-  </si>
-  <si>
-    <t>Mãng cầu(4-5 trái/kg)</t>
-  </si>
-  <si>
-    <t>Gạo tẻ trắng IR 64 25% tấm</t>
-  </si>
-  <si>
-    <t>Quýt tiểu loại 1</t>
-  </si>
-  <si>
-    <t>Táo khô(trung quốc)</t>
-  </si>
-  <si>
-    <t>Nho khô loại lớn</t>
-  </si>
-  <si>
-    <t>Hạt dưa</t>
-  </si>
-  <si>
-    <t>Mứt khoai thanh</t>
-  </si>
-  <si>
-    <t>Mứt dừa dẻo</t>
-  </si>
-  <si>
-    <t>Mứt me</t>
-  </si>
-  <si>
-    <t>Mứt bí tâm</t>
-  </si>
-  <si>
-    <t>Mứt gừng huế</t>
-  </si>
-  <si>
-    <t>Mứt hạt sen huế</t>
-  </si>
-  <si>
-    <t>Mứt mãng cầu</t>
-  </si>
-  <si>
-    <t>Táo trung quốc</t>
-  </si>
-  <si>
-    <t>Lê trung quốc</t>
-  </si>
-  <si>
-    <t>Nho tươi đỏ(mỹ)</t>
-  </si>
-  <si>
-    <t>Bánh hộp kinh đô 500 gr</t>
-  </si>
-  <si>
-    <t>Bánh hộp Danisa 453 gr</t>
-  </si>
-  <si>
-    <t>Bánh hộp Bibica (Biên Hòa) 350 gr</t>
-  </si>
-  <si>
-    <t>Trà sen loại 1</t>
-  </si>
-  <si>
-    <t>Nước ngọt Pepsi lon (Thùng 24 lon)</t>
-  </si>
-  <si>
-    <t>Nhãn tiêu</t>
-  </si>
-  <si>
-    <t>Đu Đủ</t>
-  </si>
-  <si>
-    <t>Tôm sú</t>
-  </si>
-  <si>
-    <t>Dưa hấu giống TL trái 3 kg</t>
-  </si>
-  <si>
-    <t>Thịt Vai</t>
-  </si>
-  <si>
-    <t>Thịt nách</t>
-  </si>
-  <si>
-    <t>Thịt cốt lếch</t>
-  </si>
-  <si>
-    <t>sườn già</t>
-  </si>
-  <si>
-    <t>chân giò</t>
-  </si>
-  <si>
-    <t>Dầu ăn tổng hợp Nakydaco (chai 1 lít)</t>
-  </si>
-  <si>
-    <t>Dầu ăn tổng hợp Neptune (chai 1 lít)</t>
-  </si>
-  <si>
-    <t>chả lụa cơ sở DÌ BẢY</t>
-  </si>
-  <si>
-    <t>Dầu ăn tổng hợp TƯỜNG AN (chai 1 lit)</t>
-  </si>
-  <si>
-    <t>Chợ Gò vấp</t>
-  </si>
-  <si>
-    <t>BigC Gò Vấp</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>-2</t>
@@ -449,20 +452,22 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -768,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,25 +782,25 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="38.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -807,13 +812,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="5">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -821,12 +826,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>122</v>
       </c>
     </row>
@@ -835,12 +840,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="5">
+        <v>47</v>
+      </c>
+      <c r="D5" s="2">
         <v>21</v>
       </c>
     </row>
@@ -849,13 +854,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="5">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -863,12 +868,12 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="5">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2">
         <v>10</v>
       </c>
     </row>
@@ -877,12 +882,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="5">
+        <v>47</v>
+      </c>
+      <c r="D8" s="2">
         <v>78</v>
       </c>
     </row>
@@ -891,12 +896,12 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="5">
+        <v>47</v>
+      </c>
+      <c r="D9" s="2">
         <v>100</v>
       </c>
     </row>
@@ -905,12 +910,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="5">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2">
         <v>87</v>
       </c>
     </row>
@@ -919,12 +924,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="5">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2">
         <v>35</v>
       </c>
     </row>
@@ -933,12 +938,12 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="5">
+        <v>47</v>
+      </c>
+      <c r="D12" s="2">
         <v>230</v>
       </c>
     </row>
@@ -947,12 +952,12 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="5">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2">
         <v>220</v>
       </c>
     </row>
@@ -961,12 +966,12 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="5">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2">
         <v>125</v>
       </c>
     </row>
@@ -975,12 +980,12 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="5">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2">
         <v>13</v>
       </c>
     </row>
@@ -988,13 +993,10 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="5">
+        <v>47</v>
+      </c>
+      <c r="D16" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1003,12 +1005,12 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="5">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2">
         <v>28</v>
       </c>
     </row>
@@ -1017,12 +1019,12 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="5">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2">
         <v>36</v>
       </c>
     </row>
@@ -1031,12 +1033,12 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="5">
+        <v>47</v>
+      </c>
+      <c r="D19" s="2">
         <v>100</v>
       </c>
     </row>
@@ -1045,12 +1047,12 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="5">
+        <v>47</v>
+      </c>
+      <c r="D20" s="2">
         <v>150</v>
       </c>
     </row>
@@ -1059,12 +1061,12 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="5">
+        <v>47</v>
+      </c>
+      <c r="D21" s="2">
         <v>620</v>
       </c>
     </row>
@@ -1073,12 +1075,12 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="5">
+        <v>47</v>
+      </c>
+      <c r="D22" s="2">
         <v>43</v>
       </c>
     </row>
@@ -1087,12 +1089,12 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="5">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2">
         <v>26</v>
       </c>
     </row>
@@ -1101,12 +1103,12 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="5">
+        <v>47</v>
+      </c>
+      <c r="D24" s="2">
         <v>17</v>
       </c>
     </row>
@@ -1115,12 +1117,12 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="5">
+        <v>47</v>
+      </c>
+      <c r="D25" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1129,12 +1131,12 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="5">
+        <v>47</v>
+      </c>
+      <c r="D26" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1143,12 +1145,12 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="5">
+        <v>47</v>
+      </c>
+      <c r="D27" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1157,12 +1159,12 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="5">
+        <v>47</v>
+      </c>
+      <c r="D28" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1171,12 +1173,12 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="5">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1185,12 +1187,12 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="5">
+        <v>47</v>
+      </c>
+      <c r="D30" s="2">
         <v>50</v>
       </c>
     </row>
@@ -1199,12 +1201,12 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="5">
+        <v>47</v>
+      </c>
+      <c r="D31" s="2">
         <v>18</v>
       </c>
     </row>
@@ -1213,12 +1215,12 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="5">
+        <v>47</v>
+      </c>
+      <c r="D32" s="2">
         <v>65</v>
       </c>
     </row>
@@ -1227,12 +1229,12 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="5">
+        <v>47</v>
+      </c>
+      <c r="D33" s="2">
         <v>19</v>
       </c>
     </row>
@@ -1241,12 +1243,12 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="5">
+        <v>47</v>
+      </c>
+      <c r="D34" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1255,12 +1257,12 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="5">
+        <v>47</v>
+      </c>
+      <c r="D35" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1269,12 +1271,12 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="5">
+        <v>47</v>
+      </c>
+      <c r="D36" s="2">
         <v>17</v>
       </c>
     </row>
@@ -1283,12 +1285,12 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="5">
+        <v>47</v>
+      </c>
+      <c r="D37" s="2">
         <v>58</v>
       </c>
     </row>
@@ -1297,12 +1299,12 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="5">
+        <v>47</v>
+      </c>
+      <c r="D38" s="2">
         <v>100</v>
       </c>
     </row>
@@ -1311,12 +1313,12 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="5">
+        <v>47</v>
+      </c>
+      <c r="D39" s="2">
         <v>70</v>
       </c>
     </row>
@@ -1325,12 +1327,12 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="5">
+        <v>47</v>
+      </c>
+      <c r="D40" s="2">
         <v>165</v>
       </c>
     </row>
@@ -1339,12 +1341,12 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="5">
+        <v>47</v>
+      </c>
+      <c r="D41" s="2">
         <v>265</v>
       </c>
     </row>
@@ -1353,12 +1355,12 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="5">
+        <v>47</v>
+      </c>
+      <c r="D42" s="2">
         <v>360</v>
       </c>
     </row>
@@ -1367,12 +1369,12 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="5">
+        <v>47</v>
+      </c>
+      <c r="D43" s="2">
         <v>12</v>
       </c>
     </row>
@@ -1381,12 +1383,12 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="5">
+        <v>47</v>
+      </c>
+      <c r="D44" s="2">
         <v>28</v>
       </c>
     </row>
@@ -1395,12 +1397,12 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="5">
+        <v>47</v>
+      </c>
+      <c r="D45" s="2">
         <v>30</v>
       </c>
     </row>
@@ -1409,13 +1411,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>119</v>
+        <v>47</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,12 +1425,12 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="5">
+        <v>47</v>
+      </c>
+      <c r="D47" s="2">
         <v>650</v>
       </c>
     </row>
@@ -1437,12 +1439,12 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="5">
+        <v>47</v>
+      </c>
+      <c r="D48" s="2">
         <v>33</v>
       </c>
     </row>
@@ -1451,13 +1453,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>120</v>
+        <v>47</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1465,12 +1467,12 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="5">
+        <v>47</v>
+      </c>
+      <c r="D50" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1479,12 +1481,12 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="5">
+        <v>47</v>
+      </c>
+      <c r="D51" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1493,12 +1495,12 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="5">
+        <v>47</v>
+      </c>
+      <c r="D52" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1507,13 +1509,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>118</v>
+        <v>47</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,12 +1523,12 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="5">
+        <v>47</v>
+      </c>
+      <c r="D54" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1535,12 +1537,12 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="5">
+        <v>47</v>
+      </c>
+      <c r="D55" s="2">
         <v>200</v>
       </c>
     </row>
@@ -1549,12 +1551,12 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D56" s="5">
+        <v>47</v>
+      </c>
+      <c r="D56" s="2">
         <v>65</v>
       </c>
     </row>
@@ -1563,12 +1565,12 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="5">
+        <v>47</v>
+      </c>
+      <c r="D57" s="2">
         <v>50</v>
       </c>
     </row>
@@ -1577,12 +1579,12 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="5">
+        <v>47</v>
+      </c>
+      <c r="D58" s="2">
         <v>17</v>
       </c>
     </row>
@@ -1591,12 +1593,12 @@
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="5">
+        <v>47</v>
+      </c>
+      <c r="D59" s="2">
         <v>87</v>
       </c>
     </row>
@@ -1605,12 +1607,12 @@
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="5">
+        <v>47</v>
+      </c>
+      <c r="D60" s="2">
         <v>60</v>
       </c>
     </row>
@@ -1619,12 +1621,12 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D61" s="5">
+        <v>47</v>
+      </c>
+      <c r="D61" s="2">
         <v>60</v>
       </c>
     </row>
@@ -1633,12 +1635,12 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" s="5">
+        <v>47</v>
+      </c>
+      <c r="D62" s="2">
         <v>90</v>
       </c>
     </row>
@@ -1647,12 +1649,12 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="5">
+        <v>47</v>
+      </c>
+      <c r="D63" s="2">
         <v>100</v>
       </c>
     </row>
@@ -1661,12 +1663,12 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" s="5">
+        <v>47</v>
+      </c>
+      <c r="D64" s="2">
         <v>150</v>
       </c>
     </row>
@@ -1675,12 +1677,12 @@
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D65" s="5">
+        <v>47</v>
+      </c>
+      <c r="D65" s="2">
         <v>150</v>
       </c>
     </row>
@@ -1689,12 +1691,12 @@
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D66" s="5">
+        <v>47</v>
+      </c>
+      <c r="D66" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1703,12 +1705,12 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D67" s="5">
+        <v>47</v>
+      </c>
+      <c r="D67" s="2">
         <v>12</v>
       </c>
     </row>
@@ -1717,12 +1719,12 @@
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D68" s="5">
+        <v>47</v>
+      </c>
+      <c r="D68" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1731,12 +1733,12 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D69" s="5">
+        <v>47</v>
+      </c>
+      <c r="D69" s="2">
         <v>18</v>
       </c>
     </row>
@@ -1745,12 +1747,12 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70" s="5">
+        <v>47</v>
+      </c>
+      <c r="D70" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1759,12 +1761,12 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71" s="5">
+        <v>47</v>
+      </c>
+      <c r="D71" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1773,12 +1775,12 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D72" s="5">
+        <v>47</v>
+      </c>
+      <c r="D72" s="2">
         <v>35</v>
       </c>
     </row>
@@ -1787,12 +1789,12 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D73" s="5">
+        <v>47</v>
+      </c>
+      <c r="D73" s="2">
         <v>50</v>
       </c>
     </row>
@@ -1801,13 +1803,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>121</v>
+        <v>47</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1815,12 +1817,12 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D75" s="5">
+        <v>47</v>
+      </c>
+      <c r="D75" s="2">
         <v>30</v>
       </c>
     </row>
@@ -1829,12 +1831,12 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D76" s="5">
+        <v>47</v>
+      </c>
+      <c r="D76" s="2">
         <v>130</v>
       </c>
     </row>
@@ -1843,12 +1845,12 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" s="5">
+        <v>47</v>
+      </c>
+      <c r="D77" s="2">
         <v>190</v>
       </c>
     </row>
@@ -1857,12 +1859,12 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D78" s="5">
+        <v>47</v>
+      </c>
+      <c r="D78" s="2">
         <v>22</v>
       </c>
     </row>
@@ -1871,12 +1873,12 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="5">
+        <v>47</v>
+      </c>
+      <c r="D79" s="2">
         <v>50</v>
       </c>
     </row>
@@ -1885,12 +1887,12 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D80" s="5">
+        <v>47</v>
+      </c>
+      <c r="D80" s="2">
         <v>12</v>
       </c>
     </row>
@@ -1899,12 +1901,12 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D81" s="5">
+        <v>47</v>
+      </c>
+      <c r="D81" s="2">
         <v>60</v>
       </c>
     </row>
@@ -1913,12 +1915,12 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D82" s="5">
+        <v>47</v>
+      </c>
+      <c r="D82" s="2">
         <v>70</v>
       </c>
     </row>
@@ -1927,12 +1929,12 @@
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D83" s="5">
+        <v>47</v>
+      </c>
+      <c r="D83" s="2">
         <v>105</v>
       </c>
     </row>
@@ -1941,12 +1943,12 @@
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D84" s="5">
+        <v>47</v>
+      </c>
+      <c r="D84" s="2">
         <v>68</v>
       </c>
     </row>
@@ -1955,12 +1957,12 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="5">
+        <v>47</v>
+      </c>
+      <c r="D85" s="2">
         <v>40</v>
       </c>
     </row>
@@ -1969,12 +1971,12 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D86" s="5">
+        <v>47</v>
+      </c>
+      <c r="D86" s="2">
         <v>95</v>
       </c>
     </row>
@@ -1983,12 +1985,12 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D87" s="5">
+        <v>47</v>
+      </c>
+      <c r="D87" s="2">
         <v>75</v>
       </c>
     </row>
@@ -1997,12 +1999,12 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D88" s="5">
+        <v>47</v>
+      </c>
+      <c r="D88" s="2">
         <v>45</v>
       </c>
     </row>
@@ -2011,12 +2013,12 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D89" s="5">
+        <v>47</v>
+      </c>
+      <c r="D89" s="2">
         <v>70</v>
       </c>
     </row>
@@ -2025,12 +2027,12 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D90" s="5">
+        <v>47</v>
+      </c>
+      <c r="D90" s="2">
         <v>100</v>
       </c>
     </row>
@@ -2039,12 +2041,12 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D91" s="5">
+        <v>47</v>
+      </c>
+      <c r="D91" s="2">
         <v>80</v>
       </c>
     </row>
@@ -2053,12 +2055,12 @@
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D92" s="5">
+        <v>47</v>
+      </c>
+      <c r="D92" s="2">
         <v>40</v>
       </c>
     </row>
@@ -2067,12 +2069,12 @@
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D93" s="5">
+        <v>47</v>
+      </c>
+      <c r="D93" s="2">
         <v>30</v>
       </c>
     </row>
@@ -2081,12 +2083,12 @@
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D94" s="5">
+        <v>47</v>
+      </c>
+      <c r="D94" s="2">
         <v>100</v>
       </c>
     </row>
@@ -2095,12 +2097,12 @@
         <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D95" s="5">
+        <v>47</v>
+      </c>
+      <c r="D95" s="2">
         <v>80</v>
       </c>
     </row>
@@ -2109,12 +2111,12 @@
         <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D96" s="5">
+        <v>47</v>
+      </c>
+      <c r="D96" s="2">
         <v>90</v>
       </c>
     </row>
@@ -2123,12 +2125,12 @@
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D97" s="5">
+        <v>47</v>
+      </c>
+      <c r="D97" s="2">
         <v>55</v>
       </c>
     </row>
@@ -2137,12 +2139,12 @@
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D98" s="5">
+        <v>47</v>
+      </c>
+      <c r="D98" s="2">
         <v>120</v>
       </c>
     </row>
@@ -2151,12 +2153,12 @@
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D99" s="5">
+        <v>47</v>
+      </c>
+      <c r="D99" s="2">
         <v>152</v>
       </c>
     </row>
@@ -2165,12 +2167,12 @@
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D100" s="5">
+        <v>47</v>
+      </c>
+      <c r="D100" s="2">
         <v>25</v>
       </c>
     </row>
@@ -2179,12 +2181,12 @@
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D101" s="5">
+        <v>47</v>
+      </c>
+      <c r="D101" s="2">
         <v>15</v>
       </c>
     </row>
@@ -2193,12 +2195,12 @@
         <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D102" s="5">
+        <v>47</v>
+      </c>
+      <c r="D102" s="2">
         <v>60</v>
       </c>
     </row>
@@ -2207,12 +2209,12 @@
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D103" s="5">
+        <v>47</v>
+      </c>
+      <c r="D103" s="2">
         <v>9</v>
       </c>
     </row>
@@ -2221,12 +2223,12 @@
         <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D104" s="5">
+        <v>47</v>
+      </c>
+      <c r="D104" s="2">
         <v>70</v>
       </c>
     </row>
@@ -2235,12 +2237,12 @@
         <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D105" s="5">
+        <v>47</v>
+      </c>
+      <c r="D105" s="2">
         <v>72</v>
       </c>
     </row>
@@ -2249,12 +2251,12 @@
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D106" s="5">
+        <v>47</v>
+      </c>
+      <c r="D106" s="2">
         <v>82</v>
       </c>
     </row>
@@ -2263,12 +2265,12 @@
         <v>105</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D107" s="5">
+        <v>47</v>
+      </c>
+      <c r="D107" s="2">
         <v>80</v>
       </c>
     </row>
@@ -2277,12 +2279,12 @@
         <v>106</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D108" s="5">
+        <v>47</v>
+      </c>
+      <c r="D108" s="2">
         <v>70</v>
       </c>
     </row>
@@ -2291,12 +2293,12 @@
         <v>107</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D109" s="5">
+        <v>47</v>
+      </c>
+      <c r="D109" s="2">
         <v>42</v>
       </c>
     </row>
@@ -2305,12 +2307,12 @@
         <v>108</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D110" s="5">
+        <v>47</v>
+      </c>
+      <c r="D110" s="2">
         <v>40</v>
       </c>
     </row>
@@ -2319,12 +2321,12 @@
         <v>109</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D111" s="5">
+        <v>47</v>
+      </c>
+      <c r="D111" s="2">
         <v>150</v>
       </c>
     </row>
@@ -2333,16 +2335,17 @@
         <v>110</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D112" s="5">
+        <v>47</v>
+      </c>
+      <c r="D112" s="2">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CC1A" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>

</xml_diff>